<commit_message>
Deploying to gh-pages from @ joaobtj/boletim_inmet@88d721f79c1341bac99bf3f75607dae851a736e0 🚀
</commit_message>
<xml_diff>
--- a/estacoes.xlsx
+++ b/estacoes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ufscbr-my.sharepoint.com/personal/joao_tolentino_ufsc_br/Documents/GitLab/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ufscbr-my.sharepoint.com/personal/joao_tolentino_ufsc_br/Documents/GitLab/boletim_inmet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B0A3EF54-74A4-4B64-A1C7-0D8C8771194F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:40009_{B0A3EF54-74A4-4B64-A1C7-0D8C8771194F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7ED30D11-8A8C-4BC2-93AA-C670919B6441}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CatalogoEstaçõesAutomáticas" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CatalogoEstaçõesAutomáticas!$A$1:$H$572</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">SC!$A$1:$H$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -3560,7 +3561,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4395,7 +4396,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:H572"/>
   <sheetViews>
@@ -19288,7 +19289,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H572">
+  <autoFilter ref="A1:H572" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="1">
       <filters>
         <filter val="SC"/>
@@ -19303,11 +19304,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19947,6 +19948,11 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H1" xr:uid="{00000000-0001-0000-0100-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H24">
+      <sortCondition ref="G1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Deploying to gh-pages from @ joaobtj/boletim_inmet@9bb9fc6db1ac9c05ffa61900bb67c0d4e7327e92 🚀
</commit_message>
<xml_diff>
--- a/estacoes.xlsx
+++ b/estacoes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ufscbr-my.sharepoint.com/personal/joao_tolentino_ufsc_br/Documents/GitLab/boletim_inmet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:40009_{B0A3EF54-74A4-4B64-A1C7-0D8C8771194F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7ED30D11-8A8C-4BC2-93AA-C670919B6441}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:40009_{B0A3EF54-74A4-4B64-A1C7-0D8C8771194F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4772EE9-4178-46DF-8EE9-07207502F84F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CatalogoEstaçõesAutomáticas" sheetId="1" r:id="rId1"/>
@@ -4400,8 +4400,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:H572"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H570"/>
+    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="D489" sqref="D489"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4676,7 +4676,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -5352,7 +5352,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>428</v>
       </c>
@@ -5612,7 +5612,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>123</v>
       </c>
@@ -6184,7 +6184,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>167</v>
       </c>
@@ -6288,7 +6288,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>504</v>
       </c>
@@ -6704,7 +6704,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>538</v>
       </c>
@@ -6730,7 +6730,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>210</v>
       </c>
@@ -6912,7 +6912,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>224</v>
       </c>
@@ -6964,7 +6964,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>228</v>
       </c>
@@ -7120,7 +7120,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="105" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>241</v>
       </c>
@@ -7354,7 +7354,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>176</v>
       </c>
@@ -7406,7 +7406,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>263</v>
       </c>
@@ -7432,7 +7432,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>265</v>
       </c>
@@ -7484,7 +7484,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>269</v>
       </c>
@@ -8030,7 +8030,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>587</v>
       </c>
@@ -8602,7 +8602,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="162" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>355</v>
       </c>
@@ -8758,7 +8758,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>368</v>
       </c>
@@ -8914,7 +8914,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>557</v>
       </c>
@@ -9018,7 +9018,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="178" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>388</v>
       </c>
@@ -9226,7 +9226,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="186" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>404</v>
       </c>
@@ -9278,7 +9278,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="188" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>408</v>
       </c>
@@ -9538,7 +9538,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>907</v>
       </c>
@@ -9720,7 +9720,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="205" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>442</v>
       </c>
@@ -10292,7 +10292,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="227" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>486</v>
       </c>
@@ -10526,7 +10526,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>1017</v>
       </c>
@@ -10968,7 +10968,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="253" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>1171</v>
       </c>
@@ -11202,7 +11202,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="262" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>208</v>
       </c>
@@ -11332,7 +11332,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="267" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>567</v>
       </c>
@@ -11592,7 +11592,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="277" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>911</v>
       </c>
@@ -11852,7 +11852,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="287" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>995</v>
       </c>
@@ -11904,7 +11904,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="289" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>611</v>
       </c>
@@ -12086,7 +12086,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="296" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>1140</v>
       </c>
@@ -12268,7 +12268,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="303" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>380</v>
       </c>
@@ -13126,7 +13126,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="336" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
         <v>705</v>
       </c>
@@ -13464,7 +13464,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="349" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
         <v>625</v>
       </c>
@@ -13776,7 +13776,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="361" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
         <v>755</v>
       </c>
@@ -14192,7 +14192,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="377" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A377" t="s">
         <v>787</v>
       </c>
@@ -14868,7 +14868,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="403" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A403" t="s">
         <v>839</v>
       </c>
@@ -15258,7 +15258,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="418" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A418" t="s">
         <v>869</v>
       </c>
@@ -15388,7 +15388,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="423" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A423" t="s">
         <v>731</v>
       </c>
@@ -15752,7 +15752,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="437" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A437" t="s">
         <v>98</v>
       </c>
@@ -15778,7 +15778,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="438" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A438" t="s">
         <v>909</v>
       </c>
@@ -15804,7 +15804,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="439" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A439" t="s">
         <v>639</v>
       </c>
@@ -15830,7 +15830,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="440" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A440" t="s">
         <v>913</v>
       </c>
@@ -16324,7 +16324,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="459" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="459" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A459" t="s">
         <v>951</v>
       </c>
@@ -16428,7 +16428,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="463" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="463" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A463" t="s">
         <v>959</v>
       </c>
@@ -16532,7 +16532,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="467" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="467" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A467" t="s">
         <v>967</v>
       </c>
@@ -16584,7 +16584,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="469" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="469" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A469" t="s">
         <v>971</v>
       </c>
@@ -16636,7 +16636,7 @@
         <v>974</v>
       </c>
     </row>
-    <row r="471" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="471" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A471" t="s">
         <v>975</v>
       </c>
@@ -16662,7 +16662,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="472" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="472" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A472" t="s">
         <v>977</v>
       </c>
@@ -16766,7 +16766,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="476" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="476" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A476" t="s">
         <v>985</v>
       </c>
@@ -16896,7 +16896,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="481" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="481" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A481" t="s">
         <v>607</v>
       </c>
@@ -16948,7 +16948,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="483" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="483" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A483" t="s">
         <v>999</v>
       </c>
@@ -17052,7 +17052,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="487" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="487" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A487" t="s">
         <v>1007</v>
       </c>
@@ -17182,7 +17182,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="492" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="492" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A492" t="s">
         <v>879</v>
       </c>
@@ -17416,7 +17416,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="501" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="501" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A501" t="s">
         <v>1034</v>
       </c>
@@ -17520,7 +17520,7 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="505" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="505" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A505" t="s">
         <v>1042</v>
       </c>
@@ -17884,7 +17884,7 @@
         <v>1069</v>
       </c>
     </row>
-    <row r="519" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="519" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A519" t="s">
         <v>1070</v>
       </c>
@@ -18040,7 +18040,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="525" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="525" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A525" t="s">
         <v>1082</v>
       </c>
@@ -18222,7 +18222,7 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="532" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="532" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A532" t="s">
         <v>1096</v>
       </c>
@@ -18326,7 +18326,7 @@
         <v>1103</v>
       </c>
     </row>
-    <row r="536" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="536" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A536" t="s">
         <v>1104</v>
       </c>
@@ -18352,7 +18352,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="537" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="537" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A537" t="s">
         <v>1106</v>
       </c>
@@ -18534,7 +18534,7 @@
         <v>1119</v>
       </c>
     </row>
-    <row r="544" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="544" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A544" t="s">
         <v>1120</v>
       </c>
@@ -18768,7 +18768,7 @@
         <v>1137</v>
       </c>
     </row>
-    <row r="553" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="553" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A553" t="s">
         <v>1138</v>
       </c>
@@ -18794,7 +18794,7 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="554" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="554" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A554" t="s">
         <v>259</v>
       </c>
@@ -18820,7 +18820,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="555" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="555" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A555" t="s">
         <v>1142</v>
       </c>
@@ -19210,7 +19210,7 @@
         <v>1170</v>
       </c>
     </row>
-    <row r="570" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="570" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A570" t="s">
         <v>311</v>
       </c>
@@ -19292,11 +19292,11 @@
   <autoFilter ref="A1:H572" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="1">
       <filters>
-        <filter val="SC"/>
+        <filter val="RS"/>
       </filters>
     </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A37:H570">
-      <sortCondition ref="G1:G572"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A102:H562">
+      <sortCondition ref="A1:A572"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -19307,7 +19307,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
@@ -19351,7 +19351,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>428</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
         <v>99</v>
@@ -19360,50 +19360,50 @@
         <v>17</v>
       </c>
       <c r="D2">
-        <v>-27.602530000000002</v>
+        <v>-28.931353000000001</v>
       </c>
       <c r="E2">
-        <v>-48.620095999999997</v>
+        <v>-49.497920000000001</v>
       </c>
       <c r="F2">
-        <v>4.87</v>
+        <v>2</v>
       </c>
       <c r="G2" s="1">
-        <v>37642</v>
+        <v>39718</v>
       </c>
       <c r="H2" t="s">
-        <v>429</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>504</v>
+        <v>176</v>
       </c>
       <c r="B3" t="s">
         <v>99</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D3">
-        <v>-26.913611110000002</v>
+        <v>-28.126944430000002</v>
       </c>
       <c r="E3">
-        <v>-49.268055539999999</v>
+        <v>-49.479722209999998</v>
       </c>
       <c r="F3">
-        <v>72.239999999999995</v>
+        <v>1790.38</v>
       </c>
       <c r="G3" s="1">
-        <v>38899</v>
+        <v>39249</v>
       </c>
       <c r="H3" t="s">
-        <v>505</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>538</v>
+        <v>208</v>
       </c>
       <c r="B4" t="s">
         <v>99</v>
@@ -19412,24 +19412,24 @@
         <v>17</v>
       </c>
       <c r="D4">
-        <v>-26.081388879999999</v>
+        <v>-26.819156</v>
       </c>
       <c r="E4">
-        <v>-48.641666659999999</v>
+        <v>-50.985520000000001</v>
       </c>
       <c r="F4">
-        <v>6.18</v>
+        <v>944.26</v>
       </c>
       <c r="G4" s="1">
-        <v>39238</v>
+        <v>39525</v>
       </c>
       <c r="H4" t="s">
-        <v>539</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>176</v>
+        <v>259</v>
       </c>
       <c r="B5" t="s">
         <v>99</v>
@@ -19438,24 +19438,24 @@
         <v>17</v>
       </c>
       <c r="D5">
-        <v>-28.126944430000002</v>
+        <v>-27.388611099999999</v>
       </c>
       <c r="E5">
-        <v>-49.479722209999998</v>
+        <v>-51.215833330000002</v>
       </c>
       <c r="F5">
-        <v>1790.38</v>
+        <v>963</v>
       </c>
       <c r="G5" s="1">
-        <v>39249</v>
+        <v>43510</v>
       </c>
       <c r="H5" t="s">
-        <v>177</v>
+        <v>260</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>587</v>
+        <v>311</v>
       </c>
       <c r="B6" t="s">
         <v>99</v>
@@ -19464,19 +19464,19 @@
         <v>17</v>
       </c>
       <c r="D6">
-        <v>-27.169166659999998</v>
+        <v>-27.085311099999998</v>
       </c>
       <c r="E6">
-        <v>-51.558888879999998</v>
+        <v>-52.635711100000002</v>
       </c>
       <c r="F6">
-        <v>767.63</v>
+        <v>679</v>
       </c>
       <c r="G6" s="1">
-        <v>39344</v>
+        <v>43514</v>
       </c>
       <c r="H6" t="s">
-        <v>588</v>
+        <v>312</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -19507,7 +19507,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>557</v>
+        <v>380</v>
       </c>
       <c r="B8" t="s">
         <v>99</v>
@@ -19516,24 +19516,24 @@
         <v>17</v>
       </c>
       <c r="D8">
-        <v>-27.418333319999999</v>
+        <v>-26.286562</v>
       </c>
       <c r="E8">
-        <v>-49.646944439999999</v>
+        <v>-53.633113999999999</v>
       </c>
       <c r="F8">
-        <v>479.79</v>
+        <v>807.54</v>
       </c>
       <c r="G8" s="1">
-        <v>39510</v>
+        <v>39598</v>
       </c>
       <c r="H8" t="s">
-        <v>558</v>
+        <v>381</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>907</v>
+        <v>428</v>
       </c>
       <c r="B9" t="s">
         <v>99</v>
@@ -19542,50 +19542,50 @@
         <v>17</v>
       </c>
       <c r="D9">
-        <v>-26.937499989999999</v>
+        <v>-27.602530000000002</v>
       </c>
       <c r="E9">
-        <v>-50.145555549999997</v>
+        <v>-48.620095999999997</v>
       </c>
       <c r="F9">
-        <v>591.66999999999996</v>
+        <v>4.87</v>
       </c>
       <c r="G9" s="1">
-        <v>39516</v>
+        <v>37642</v>
       </c>
       <c r="H9" t="s">
-        <v>908</v>
+        <v>429</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>1017</v>
+        <v>504</v>
       </c>
       <c r="B10" t="s">
         <v>99</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D10">
-        <v>-26.786111099999999</v>
+        <v>-26.913611110000002</v>
       </c>
       <c r="E10">
-        <v>-53.513888880000003</v>
+        <v>-49.268055539999999</v>
       </c>
       <c r="F10">
-        <v>645</v>
+        <v>72.239999999999995</v>
       </c>
       <c r="G10" s="1">
-        <v>39518</v>
+        <v>38899</v>
       </c>
       <c r="H10" t="s">
-        <v>1018</v>
+        <v>505</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>1171</v>
+        <v>538</v>
       </c>
       <c r="B11" t="s">
         <v>99</v>
@@ -19594,24 +19594,24 @@
         <v>17</v>
       </c>
       <c r="D11">
-        <v>-26.938666000000001</v>
+        <v>-26.081388879999999</v>
       </c>
       <c r="E11">
-        <v>-52.398090000000003</v>
+        <v>-48.641666659999999</v>
       </c>
       <c r="F11">
-        <v>878.74</v>
+        <v>6.18</v>
       </c>
       <c r="G11" s="1">
-        <v>39521</v>
+        <v>39238</v>
       </c>
       <c r="H11" t="s">
-        <v>1172</v>
+        <v>539</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>208</v>
+        <v>557</v>
       </c>
       <c r="B12" t="s">
         <v>99</v>
@@ -19620,24 +19620,24 @@
         <v>17</v>
       </c>
       <c r="D12">
-        <v>-26.819156</v>
+        <v>-27.418333319999999</v>
       </c>
       <c r="E12">
-        <v>-50.985520000000001</v>
+        <v>-49.646944439999999</v>
       </c>
       <c r="F12">
-        <v>944.26</v>
+        <v>479.79</v>
       </c>
       <c r="G12" s="1">
-        <v>39525</v>
+        <v>39510</v>
       </c>
       <c r="H12" t="s">
-        <v>209</v>
+        <v>558</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>911</v>
+        <v>587</v>
       </c>
       <c r="B13" t="s">
         <v>99</v>
@@ -19646,24 +19646,24 @@
         <v>17</v>
       </c>
       <c r="D13">
-        <v>-26.248611100000002</v>
+        <v>-27.169166659999998</v>
       </c>
       <c r="E13">
-        <v>-49.574166660000003</v>
+        <v>-51.558888879999998</v>
       </c>
       <c r="F13">
-        <v>800</v>
+        <v>767.63</v>
       </c>
       <c r="G13" s="1">
-        <v>39528</v>
+        <v>39344</v>
       </c>
       <c r="H13" t="s">
-        <v>912</v>
+        <v>588</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>995</v>
+        <v>607</v>
       </c>
       <c r="B14" t="s">
         <v>99</v>
@@ -19672,50 +19672,50 @@
         <v>17</v>
       </c>
       <c r="D14">
-        <v>-28.275639999999999</v>
+        <v>-27.802222220000001</v>
       </c>
       <c r="E14">
-        <v>-49.934617000000003</v>
+        <v>-50.335555550000002</v>
       </c>
       <c r="F14">
-        <v>1400.06</v>
+        <v>952.7</v>
       </c>
       <c r="G14" s="1">
-        <v>39549</v>
+        <v>41948</v>
       </c>
       <c r="H14" t="s">
-        <v>996</v>
+        <v>608</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>1140</v>
+        <v>625</v>
       </c>
       <c r="B15" t="s">
         <v>99</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D15">
-        <v>-28.532499990000002</v>
+        <v>-28.604444440000002</v>
       </c>
       <c r="E15">
-        <v>-49.315277770000002</v>
+        <v>-48.813333329999999</v>
       </c>
       <c r="F15">
-        <v>40.56</v>
+        <v>34.36</v>
       </c>
       <c r="G15" s="1">
-        <v>39596</v>
+        <v>39599</v>
       </c>
       <c r="H15" t="s">
-        <v>1141</v>
+        <v>626</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>380</v>
+        <v>639</v>
       </c>
       <c r="B16" t="s">
         <v>99</v>
@@ -19724,24 +19724,24 @@
         <v>17</v>
       </c>
       <c r="D16">
-        <v>-26.286562</v>
+        <v>-26.393611100000001</v>
       </c>
       <c r="E16">
-        <v>-53.633113999999999</v>
+        <v>-50.363333330000003</v>
       </c>
       <c r="F16">
-        <v>807.54</v>
+        <v>799.58</v>
       </c>
       <c r="G16" s="1">
-        <v>39598</v>
+        <v>39852</v>
       </c>
       <c r="H16" t="s">
-        <v>381</v>
+        <v>640</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>625</v>
+        <v>731</v>
       </c>
       <c r="B17" t="s">
         <v>99</v>
@@ -19750,50 +19750,50 @@
         <v>10</v>
       </c>
       <c r="D17">
-        <v>-28.604444440000002</v>
+        <v>-26.406388880000002</v>
       </c>
       <c r="E17">
-        <v>-48.813333329999999</v>
+        <v>-52.850277769999998</v>
       </c>
       <c r="F17">
-        <v>34.36</v>
+        <v>943.57</v>
       </c>
       <c r="G17" s="1">
-        <v>39599</v>
+        <v>39710</v>
       </c>
       <c r="H17" t="s">
-        <v>626</v>
+        <v>732</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>731</v>
+        <v>879</v>
       </c>
       <c r="B18" t="s">
         <v>99</v>
       </c>
       <c r="C18" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D18">
-        <v>-26.406388880000002</v>
+        <v>-27.678611100000001</v>
       </c>
       <c r="E18">
-        <v>-52.850277769999998</v>
+        <v>-49.041944440000002</v>
       </c>
       <c r="F18">
-        <v>943.57</v>
+        <v>881</v>
       </c>
       <c r="G18" s="1">
-        <v>39710</v>
+        <v>42520</v>
       </c>
       <c r="H18" t="s">
-        <v>732</v>
+        <v>880</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>98</v>
+        <v>907</v>
       </c>
       <c r="B19" t="s">
         <v>99</v>
@@ -19802,24 +19802,24 @@
         <v>17</v>
       </c>
       <c r="D19">
-        <v>-28.931353000000001</v>
+        <v>-26.937499989999999</v>
       </c>
       <c r="E19">
-        <v>-49.497920000000001</v>
+        <v>-50.145555549999997</v>
       </c>
       <c r="F19">
-        <v>2</v>
+        <v>591.66999999999996</v>
       </c>
       <c r="G19" s="1">
-        <v>39718</v>
+        <v>39516</v>
       </c>
       <c r="H19" t="s">
-        <v>100</v>
+        <v>908</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>639</v>
+        <v>911</v>
       </c>
       <c r="B20" t="s">
         <v>99</v>
@@ -19828,24 +19828,24 @@
         <v>17</v>
       </c>
       <c r="D20">
-        <v>-26.393611100000001</v>
+        <v>-26.248611100000002</v>
       </c>
       <c r="E20">
-        <v>-50.363333330000003</v>
+        <v>-49.574166660000003</v>
       </c>
       <c r="F20">
-        <v>799.58</v>
+        <v>800</v>
       </c>
       <c r="G20" s="1">
-        <v>39852</v>
+        <v>39528</v>
       </c>
       <c r="H20" t="s">
-        <v>640</v>
+        <v>912</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>607</v>
+        <v>995</v>
       </c>
       <c r="B21" t="s">
         <v>99</v>
@@ -19854,24 +19854,24 @@
         <v>17</v>
       </c>
       <c r="D21">
-        <v>-27.802222220000001</v>
+        <v>-28.275639999999999</v>
       </c>
       <c r="E21">
-        <v>-50.335555550000002</v>
+        <v>-49.934617000000003</v>
       </c>
       <c r="F21">
-        <v>952.7</v>
+        <v>1400.06</v>
       </c>
       <c r="G21" s="1">
-        <v>41948</v>
+        <v>39549</v>
       </c>
       <c r="H21" t="s">
-        <v>608</v>
+        <v>996</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>879</v>
+        <v>1017</v>
       </c>
       <c r="B22" t="s">
         <v>99</v>
@@ -19880,24 +19880,24 @@
         <v>17</v>
       </c>
       <c r="D22">
-        <v>-27.678611100000001</v>
+        <v>-26.786111099999999</v>
       </c>
       <c r="E22">
-        <v>-49.041944440000002</v>
+        <v>-53.513888880000003</v>
       </c>
       <c r="F22">
-        <v>881</v>
+        <v>645</v>
       </c>
       <c r="G22" s="1">
-        <v>42520</v>
+        <v>39518</v>
       </c>
       <c r="H22" t="s">
-        <v>880</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>259</v>
+        <v>1140</v>
       </c>
       <c r="B23" t="s">
         <v>99</v>
@@ -19906,24 +19906,24 @@
         <v>17</v>
       </c>
       <c r="D23">
-        <v>-27.388611099999999</v>
+        <v>-28.532499990000002</v>
       </c>
       <c r="E23">
-        <v>-51.215833330000002</v>
+        <v>-49.315277770000002</v>
       </c>
       <c r="F23">
-        <v>963</v>
+        <v>40.56</v>
       </c>
       <c r="G23" s="1">
-        <v>43510</v>
+        <v>39596</v>
       </c>
       <c r="H23" t="s">
-        <v>260</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>311</v>
+        <v>1171</v>
       </c>
       <c r="B24" t="s">
         <v>99</v>
@@ -19932,25 +19932,25 @@
         <v>17</v>
       </c>
       <c r="D24">
-        <v>-27.085311099999998</v>
+        <v>-26.938666000000001</v>
       </c>
       <c r="E24">
-        <v>-52.635711100000002</v>
+        <v>-52.398090000000003</v>
       </c>
       <c r="F24">
-        <v>679</v>
+        <v>878.74</v>
       </c>
       <c r="G24" s="1">
-        <v>43514</v>
+        <v>39521</v>
       </c>
       <c r="H24" t="s">
-        <v>312</v>
+        <v>1172</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:H1" xr:uid="{00000000-0001-0000-0100-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H24">
-      <sortCondition ref="G1"/>
+      <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
cities from excel file
</commit_message>
<xml_diff>
--- a/estacoes.xlsx
+++ b/estacoes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Catalogo" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2392" uniqueCount="1177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2396" uniqueCount="1177">
   <si>
     <t>DC_NOME</t>
   </si>
@@ -4399,8 +4399,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:H572"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D489" sqref="D489"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A209" sqref="A209:XFD209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4675,7 +4675,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -5611,7 +5611,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>123</v>
       </c>
@@ -6183,7 +6183,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>167</v>
       </c>
@@ -6729,7 +6729,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>210</v>
       </c>
@@ -6911,7 +6911,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>224</v>
       </c>
@@ -6963,7 +6963,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>228</v>
       </c>
@@ -7041,7 +7041,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="102" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>234</v>
       </c>
@@ -7119,7 +7119,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>241</v>
       </c>
@@ -7405,7 +7405,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>263</v>
       </c>
@@ -7431,7 +7431,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>265</v>
       </c>
@@ -7483,7 +7483,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>269</v>
       </c>
@@ -7873,7 +7873,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="134" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>299</v>
       </c>
@@ -8055,7 +8055,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="141" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>313</v>
       </c>
@@ -8081,7 +8081,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="142" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>315</v>
       </c>
@@ -8185,7 +8185,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="146" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>323</v>
       </c>
@@ -8601,7 +8601,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>355</v>
       </c>
@@ -8731,7 +8731,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="167" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>366</v>
       </c>
@@ -8835,7 +8835,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="171" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>374</v>
       </c>
@@ -8965,7 +8965,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="176" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>384</v>
       </c>
@@ -9017,7 +9017,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>388</v>
       </c>
@@ -9225,7 +9225,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>404</v>
       </c>
@@ -9277,7 +9277,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>408</v>
       </c>
@@ -9667,7 +9667,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="203" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>438</v>
       </c>
@@ -9719,7 +9719,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>442</v>
       </c>
@@ -9823,7 +9823,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="209" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>450</v>
       </c>
@@ -9953,7 +9953,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="214" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>460</v>
       </c>
@@ -10291,7 +10291,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>486</v>
       </c>
@@ -10369,7 +10369,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="230" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>492</v>
       </c>
@@ -10499,7 +10499,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="235" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>502</v>
       </c>
@@ -11253,7 +11253,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="264" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>561</v>
       </c>
@@ -11331,7 +11331,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="267" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>567</v>
       </c>
@@ -11487,7 +11487,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="273" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>579</v>
       </c>
@@ -11669,7 +11669,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="280" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>593</v>
       </c>
@@ -11903,7 +11903,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="289" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>611</v>
       </c>
@@ -11929,7 +11929,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="290" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>613</v>
       </c>
@@ -12293,7 +12293,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="304" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>641</v>
       </c>
@@ -12657,7 +12657,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="318" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>669</v>
       </c>
@@ -13047,7 +13047,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="333" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>699</v>
       </c>
@@ -13125,7 +13125,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="336" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>705</v>
       </c>
@@ -13281,7 +13281,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="342" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>717</v>
       </c>
@@ -13359,7 +13359,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="345" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>723</v>
       </c>
@@ -13775,7 +13775,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="361" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>755</v>
       </c>
@@ -13957,7 +13957,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="368" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>769</v>
       </c>
@@ -14191,7 +14191,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="377" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
         <v>787</v>
       </c>
@@ -14711,7 +14711,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="397" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
         <v>827</v>
       </c>
@@ -14867,7 +14867,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="403" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
         <v>839</v>
       </c>
@@ -15257,7 +15257,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="418" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
         <v>869</v>
       </c>
@@ -15777,7 +15777,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="438" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
         <v>909</v>
       </c>
@@ -15829,7 +15829,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="440" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
         <v>913</v>
       </c>
@@ -16323,7 +16323,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="459" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A459" t="s">
         <v>951</v>
       </c>
@@ -16427,7 +16427,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="463" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
         <v>959</v>
       </c>
@@ -16531,7 +16531,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="467" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A467" t="s">
         <v>967</v>
       </c>
@@ -16583,7 +16583,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="469" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A469" t="s">
         <v>971</v>
       </c>
@@ -16635,7 +16635,7 @@
         <v>974</v>
       </c>
     </row>
-    <row r="471" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A471" t="s">
         <v>975</v>
       </c>
@@ -16661,7 +16661,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="472" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A472" t="s">
         <v>977</v>
       </c>
@@ -16765,7 +16765,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="476" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A476" t="s">
         <v>985</v>
       </c>
@@ -16947,7 +16947,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="483" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A483" t="s">
         <v>999</v>
       </c>
@@ -17051,7 +17051,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="487" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
         <v>1007</v>
       </c>
@@ -17103,7 +17103,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="489" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A489" t="s">
         <v>1011</v>
       </c>
@@ -17415,7 +17415,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="501" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="501" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A501" t="s">
         <v>1034</v>
       </c>
@@ -17519,7 +17519,7 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="505" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="505" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A505" t="s">
         <v>1042</v>
       </c>
@@ -17883,7 +17883,7 @@
         <v>1069</v>
       </c>
     </row>
-    <row r="519" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="519" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A519" t="s">
         <v>1070</v>
       </c>
@@ -18039,7 +18039,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="525" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="525" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A525" t="s">
         <v>1082</v>
       </c>
@@ -18221,7 +18221,7 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="532" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="532" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A532" t="s">
         <v>1096</v>
       </c>
@@ -18325,7 +18325,7 @@
         <v>1103</v>
       </c>
     </row>
-    <row r="536" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="536" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A536" t="s">
         <v>1104</v>
       </c>
@@ -18351,7 +18351,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="537" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="537" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A537" t="s">
         <v>1106</v>
       </c>
@@ -18533,7 +18533,7 @@
         <v>1119</v>
       </c>
     </row>
-    <row r="544" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="544" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A544" t="s">
         <v>1120</v>
       </c>
@@ -18767,7 +18767,7 @@
         <v>1137</v>
       </c>
     </row>
-    <row r="553" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="553" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A553" t="s">
         <v>1138</v>
       </c>
@@ -18819,7 +18819,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="555" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="555" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A555" t="s">
         <v>1142</v>
       </c>
@@ -19001,7 +19001,7 @@
         <v>1154</v>
       </c>
     </row>
-    <row r="562" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="562" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A562" t="s">
         <v>1155</v>
       </c>
@@ -19291,7 +19291,7 @@
   <autoFilter ref="A1:H572">
     <filterColumn colId="1">
       <filters>
-        <filter val="RS"/>
+        <filter val="PR"/>
       </filters>
     </filterColumn>
     <sortState ref="A102:H562">
@@ -19304,10 +19304,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19946,6 +19946,32 @@
         <v>1172</v>
       </c>
     </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>450</v>
+      </c>
+      <c r="B25" t="s">
+        <v>235</v>
+      </c>
+      <c r="C25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25">
+        <v>-26.3986111</v>
+      </c>
+      <c r="E25">
+        <v>-51.353611110000003</v>
+      </c>
+      <c r="F25">
+        <v>1009.01</v>
+      </c>
+      <c r="G25" s="1">
+        <v>39567</v>
+      </c>
+      <c r="H25" t="s">
+        <v>451</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:H1">
     <sortState ref="A2:H24">

</xml_diff>